<commit_message>
working with water pages
</commit_message>
<xml_diff>
--- a/web_scraping/generated_resources/output/2021_05_18_report.xlsx
+++ b/web_scraping/generated_resources/output/2021_05_18_report.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="530">
   <si>
     <t xml:space="preserve">Weekly edits </t>
   </si>
@@ -1575,208 +1575,49 @@
     <t>/vloca-kennishub/Digital_twin</t>
   </si>
   <si>
-    <t>AllePaginas</t>
-  </si>
-  <si>
-    <t>{'ANPR': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/ANPR ANPR'}</t>
-  </si>
-  <si>
-    <t>{'Apache Druid': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Apache_Druid Apache Druid'}</t>
+    <t>VLOCA:B-WaterSmart</t>
+  </si>
+  <si>
+    <t>{'Architectuur': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Architectuur Architectuur'}</t>
+  </si>
+  <si>
+    <t>{'IoT': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/IoT IoT'}</t>
+  </si>
+  <si>
+    <t>{'URI': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/URI URI'}</t>
+  </si>
+  <si>
+    <t>VLOCA:DenCITY</t>
   </si>
   <si>
     <t>{'API': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/API API'}</t>
   </si>
   <si>
-    <t>{'Architectuur': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Architectuur Architectuur'}</t>
-  </si>
-  <si>
-    <t>{'Backward compatibility': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Backward_compatibility Backward compatibility'}</t>
-  </si>
-  <si>
-    <t>{'Cross-cutting': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Cross-cutting Cross-cutting'}</t>
-  </si>
-  <si>
-    <t>{'Cross-Domain': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Cross-Domain Cross-Domain'}</t>
-  </si>
-  <si>
-    <t>{'Data cataloog': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_cataloog Data cataloog'}</t>
-  </si>
-  <si>
-    <t>{'Data enrichment': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_enrichment Data enrichment'}</t>
-  </si>
-  <si>
-    <t>{'Data fusion': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_fusion Data fusion'}</t>
-  </si>
-  <si>
-    <t>{'Data Lineage': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_Lineage Data Lineage'}</t>
-  </si>
-  <si>
-    <t>{'Data Ownership': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_Ownership Data Ownership'}</t>
-  </si>
-  <si>
-    <t>{'Data protection': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_protection Data protection'}</t>
-  </si>
-  <si>
-    <t>{'Data Quality': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_Quality Data Quality'}</t>
-  </si>
-  <si>
-    <t>{'Data Scheme': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_Scheme Data Scheme'}</t>
-  </si>
-  <si>
-    <t>{'Data security': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_security Data security'}</t>
-  </si>
-  <si>
-    <t>{'Data semantiek': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_semantiek Data semantiek'}</t>
-  </si>
-  <si>
-    <t>{'Data Variety': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_Variety Data Variety'}</t>
-  </si>
-  <si>
-    <t>{'Data Velocity': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_Velocity Data Velocity'}</t>
-  </si>
-  <si>
-    <t>{'Data Veracity': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_Veracity Data Veracity'}</t>
-  </si>
-  <si>
-    <t>{'Data Volume': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Data_Volume Data Volume'}</t>
-  </si>
-  <si>
-    <t>{'Database-vs-contextbroker': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Database-vs-contextbroker Database-vs-contextbroker'}</t>
-  </si>
-  <si>
-    <t>{'Digital twin': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Digital_twin Digital twin'}</t>
-  </si>
-  <si>
-    <t>{'Edge': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Edge Edge'}</t>
-  </si>
-  <si>
-    <t>{'Five star open data': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Five_star_open_data Five star open data'}</t>
-  </si>
-  <si>
-    <t>{'Floating Car Data': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Floating_Car_Data Floating Car Data'}</t>
-  </si>
-  <si>
-    <t>{'Graph-database': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Graph-database Graph-database'}</t>
-  </si>
-  <si>
-    <t>{'ICT': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/ICT ICT'}</t>
-  </si>
-  <si>
-    <t>{'InfluxDB': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/InfluxDB InfluxDB'}</t>
-  </si>
-  <si>
-    <t>{'IoT': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/IoT IoT'}</t>
-  </si>
-  <si>
-    <t>{'Knowledge graph': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Knowledge_graph Knowledge graph'}</t>
-  </si>
-  <si>
-    <t>{'Legacy': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Legacy Legacy'}</t>
-  </si>
-  <si>
-    <t>{'Linked open data': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Linked_open_data Linked open data'}</t>
-  </si>
-  <si>
-    <t>{'LoRaWAN': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/LoRaWAN LoRaWAN'}</t>
-  </si>
-  <si>
-    <t>{'NB-IOT': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/NB-IOT NB-IOT'}</t>
-  </si>
-  <si>
-    <t>{'No-sql': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/No-sql No-sql'}</t>
-  </si>
-  <si>
-    <t>{'Ontologie': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Ontologie Ontologie'}</t>
-  </si>
-  <si>
-    <t>{'Open slimme stad': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Open_slimme_stad Open slimme stad'}</t>
-  </si>
-  <si>
-    <t>{'Open urban digital twins': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Open_urban_digital_twins Open urban digital twins'}</t>
-  </si>
-  <si>
     <t>{'PostGIS': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/PostGIS PostGIS'}</t>
   </si>
   <si>
     <t>{'Postgres': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Postgres Postgres'}</t>
   </si>
   <si>
-    <t>{'Pub-sub': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Pub-sub Pub-sub'}</t>
-  </si>
-  <si>
-    <t>{'Relational-database': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Relational-database Relational-database'}</t>
-  </si>
-  <si>
     <t>{'REST-API': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/REST-API REST-API'}</t>
   </si>
   <si>
-    <t>{'Sigfox': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Sigfox Sigfox'}</t>
-  </si>
-  <si>
-    <t>{'Slimme Camera': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Slimme_Camera Slimme Camera'}</t>
-  </si>
-  <si>
-    <t>{'Slimme stad': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Slimme_stad Slimme stad'}</t>
-  </si>
-  <si>
-    <t>{'Slimme Verkeerslichten': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Slimme_Verkeerslichten Slimme Verkeerslichten'}</t>
-  </si>
-  <si>
-    <t>{'Solid': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Solid Solid'}</t>
-  </si>
-  <si>
-    <t>{'Swagger': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Swagger Swagger'}</t>
-  </si>
-  <si>
-    <t>{'Syntax': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Syntax Syntax'}</t>
-  </si>
-  <si>
-    <t>{'Telecom': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Telecom Telecom'}</t>
-  </si>
-  <si>
-    <t>{'Tellus': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Tellus Tellus'}</t>
-  </si>
-  <si>
-    <t>{'Timescale Postgres': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/Timescale_Postgres Timescale Postgres'}</t>
-  </si>
-  <si>
-    <t>{'URI': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/URI URI'}</t>
-  </si>
-  <si>
-    <t>{'WiFi scanning': 'https://vloca-kennishub.vlaanderen.be/vloca-kennishub/WiFi_scanning WiFi scanning'}</t>
-  </si>
-  <si>
-    <t>Categorieen</t>
-  </si>
-  <si>
-    <t>InhoudelijkePaginas</t>
-  </si>
-  <si>
-    <t>PopulairePaginas</t>
-  </si>
-  <si>
-    <t>RecenteWijzigingen</t>
-  </si>
-  <si>
-    <t>Standaarden</t>
-  </si>
-  <si>
-    <t>Statistieken</t>
-  </si>
-  <si>
-    <t>Technische_principes</t>
-  </si>
-  <si>
-    <t>Termen_en_Concepten</t>
-  </si>
-  <si>
-    <t>WaterPagesHome</t>
-  </si>
-  <si>
-    <t>WaterSmart</t>
-  </si>
-  <si>
-    <t>Weespaginas</t>
+    <t>VLOCA:Flood4Cast</t>
+  </si>
+  <si>
+    <t>VLOCA:Hydrologisch meetnet provincie Antwerpen</t>
+  </si>
+  <si>
+    <t>VLOCA:Koppeling IoT-peilsensordata naar andere IoT- stacks</t>
+  </si>
+  <si>
+    <t>VLOCA:Monitoring van de Laak (VLAIO CoT)</t>
+  </si>
+  <si>
+    <t>VLOCA:Nuttige water links</t>
+  </si>
+  <si>
+    <t>VLOCA:Uitleg cocreatie VLOCA traject</t>
   </si>
 </sst>
 </file>
@@ -4524,1153 +4365,191 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>515</v>
       </c>
       <c r="B1" t="s">
-        <v>572</v>
+        <v>519</v>
       </c>
       <c r="C1" t="s">
-        <v>573</v>
+        <v>316</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>524</v>
       </c>
       <c r="E1" t="s">
-        <v>169</v>
+        <v>525</v>
       </c>
       <c r="F1" t="s">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="G1" t="s">
-        <v>574</v>
+        <v>526</v>
       </c>
       <c r="H1" t="s">
-        <v>575</v>
+        <v>527</v>
       </c>
       <c r="I1" t="s">
-        <v>576</v>
+        <v>528</v>
       </c>
       <c r="J1" t="s">
-        <v>577</v>
+        <v>293</v>
       </c>
       <c r="K1" t="s">
-        <v>578</v>
+        <v>313</v>
       </c>
       <c r="L1" t="s">
-        <v>579</v>
+        <v>529</v>
       </c>
       <c r="M1" t="s">
-        <v>580</v>
+        <v>287</v>
       </c>
       <c r="N1" t="s">
-        <v>581</v>
-      </c>
-      <c r="O1" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>516</v>
       </c>
       <c r="B2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C2" t="s">
         <v>516</v>
       </c>
       <c r="D2" t="s">
+        <v>520</v>
+      </c>
+      <c r="E2" t="s">
         <v>516</v>
       </c>
-      <c r="E2" t="s">
-        <v>518</v>
-      </c>
       <c r="F2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G2" t="s">
+        <v>520</v>
+      </c>
+      <c r="H2" t="s">
         <v>516</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>516</v>
       </c>
-      <c r="H2" t="s">
-        <v>519</v>
-      </c>
-      <c r="I2" t="s">
-        <v>518</v>
-      </c>
       <c r="J2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="K2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="L2" t="s">
         <v>516</v>
       </c>
       <c r="M2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="N2" t="s">
-        <v>519</v>
-      </c>
-      <c r="O2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>517</v>
       </c>
       <c r="B3" t="s">
-        <v>570</v>
+        <v>516</v>
       </c>
       <c r="C3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D3" t="s">
+        <v>516</v>
+      </c>
+      <c r="E3" t="s">
         <v>517</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>516</v>
+      </c>
+      <c r="G3" t="s">
+        <v>516</v>
+      </c>
+      <c r="H3" t="s">
         <v>517</v>
       </c>
-      <c r="E3" t="s">
-        <v>519</v>
-      </c>
-      <c r="F3" t="s">
-        <v>517</v>
-      </c>
-      <c r="G3" t="s">
-        <v>517</v>
-      </c>
-      <c r="H3" t="s">
-        <v>570</v>
-      </c>
       <c r="I3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J3" t="s">
-        <v>554</v>
+        <v>518</v>
       </c>
       <c r="K3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L3" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="M3" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="N3" t="s">
-        <v>545</v>
-      </c>
-      <c r="O3" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>518</v>
       </c>
-      <c r="C4" t="s">
-        <v>518</v>
+      <c r="B4" t="s">
+        <v>517</v>
       </c>
       <c r="D4" t="s">
         <v>518</v>
       </c>
       <c r="E4" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F4" t="s">
         <v>518</v>
       </c>
       <c r="G4" t="s">
+        <v>517</v>
+      </c>
+      <c r="H4" t="s">
         <v>518</v>
       </c>
-      <c r="I4" t="s">
-        <v>570</v>
-      </c>
-      <c r="J4" t="s">
-        <v>570</v>
-      </c>
-      <c r="K4" t="s">
-        <v>570</v>
-      </c>
-      <c r="L4" t="s">
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" t="s">
+        <v>521</v>
+      </c>
+      <c r="G5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" t="s">
+        <v>522</v>
+      </c>
+      <c r="G6" t="s">
         <v>518</v>
       </c>
-      <c r="M4" t="s">
-        <v>570</v>
-      </c>
-      <c r="N4" t="s">
-        <v>570</v>
-      </c>
-      <c r="O4" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
-        <v>519</v>
-      </c>
-      <c r="C5" t="s">
-        <v>519</v>
-      </c>
-      <c r="D5" t="s">
-        <v>519</v>
-      </c>
-      <c r="E5" t="s">
-        <v>543</v>
-      </c>
-      <c r="F5" t="s">
-        <v>519</v>
-      </c>
-      <c r="G5" t="s">
-        <v>519</v>
-      </c>
-      <c r="L5" t="s">
-        <v>519</v>
-      </c>
-      <c r="O5" t="s">
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
-        <v>520</v>
-      </c>
-      <c r="C6" t="s">
-        <v>520</v>
-      </c>
-      <c r="D6" t="s">
-        <v>540</v>
-      </c>
-      <c r="E6" t="s">
-        <v>545</v>
-      </c>
-      <c r="F6" t="s">
-        <v>520</v>
-      </c>
-      <c r="G6" t="s">
-        <v>520</v>
-      </c>
-      <c r="L6" t="s">
-        <v>520</v>
-      </c>
-      <c r="O6" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
-        <v>521</v>
-      </c>
-      <c r="C7" t="s">
-        <v>521</v>
-      </c>
-      <c r="D7" t="s">
-        <v>541</v>
-      </c>
-      <c r="E7" t="s">
-        <v>548</v>
-      </c>
-      <c r="F7" t="s">
-        <v>523</v>
-      </c>
-      <c r="G7" t="s">
-        <v>521</v>
-      </c>
-      <c r="L7" t="s">
-        <v>521</v>
-      </c>
-      <c r="O7" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>522</v>
-      </c>
-      <c r="C8" t="s">
-        <v>522</v>
-      </c>
-      <c r="D8" t="s">
-        <v>542</v>
-      </c>
-      <c r="E8" t="s">
-        <v>552</v>
-      </c>
-      <c r="F8" t="s">
-        <v>524</v>
-      </c>
-      <c r="G8" t="s">
-        <v>522</v>
-      </c>
-      <c r="L8" t="s">
-        <v>522</v>
-      </c>
-      <c r="O8" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>523</v>
-      </c>
-      <c r="C9" t="s">
-        <v>523</v>
-      </c>
-      <c r="D9" t="s">
-        <v>544</v>
-      </c>
-      <c r="E9" t="s">
-        <v>559</v>
-      </c>
-      <c r="F9" t="s">
-        <v>526</v>
-      </c>
-      <c r="G9" t="s">
-        <v>523</v>
-      </c>
-      <c r="L9" t="s">
-        <v>523</v>
-      </c>
-      <c r="O9" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>524</v>
-      </c>
-      <c r="C10" t="s">
-        <v>524</v>
-      </c>
-      <c r="D10" t="s">
-        <v>547</v>
-      </c>
-      <c r="E10" t="s">
-        <v>570</v>
-      </c>
-      <c r="F10" t="s">
-        <v>527</v>
-      </c>
-      <c r="G10" t="s">
-        <v>524</v>
-      </c>
-      <c r="L10" t="s">
-        <v>524</v>
-      </c>
-      <c r="O10" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>525</v>
-      </c>
-      <c r="C11" t="s">
-        <v>525</v>
-      </c>
-      <c r="D11" t="s">
-        <v>549</v>
-      </c>
-      <c r="F11" t="s">
-        <v>528</v>
-      </c>
-      <c r="G11" t="s">
-        <v>525</v>
-      </c>
-      <c r="L11" t="s">
-        <v>525</v>
-      </c>
-      <c r="O11" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" t="s">
-        <v>526</v>
-      </c>
-      <c r="C12" t="s">
-        <v>526</v>
-      </c>
-      <c r="D12" t="s">
-        <v>550</v>
-      </c>
-      <c r="F12" t="s">
-        <v>529</v>
-      </c>
-      <c r="G12" t="s">
-        <v>526</v>
-      </c>
-      <c r="L12" t="s">
-        <v>526</v>
-      </c>
-      <c r="O12" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" t="s">
-        <v>527</v>
-      </c>
-      <c r="C13" t="s">
-        <v>527</v>
-      </c>
-      <c r="D13" t="s">
-        <v>551</v>
-      </c>
-      <c r="F13" t="s">
-        <v>530</v>
-      </c>
-      <c r="G13" t="s">
-        <v>527</v>
-      </c>
-      <c r="L13" t="s">
-        <v>527</v>
-      </c>
-      <c r="O13" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" t="s">
-        <v>528</v>
-      </c>
-      <c r="C14" t="s">
-        <v>528</v>
-      </c>
-      <c r="D14" t="s">
-        <v>555</v>
-      </c>
-      <c r="F14" t="s">
-        <v>531</v>
-      </c>
-      <c r="G14" t="s">
-        <v>528</v>
-      </c>
-      <c r="L14" t="s">
-        <v>528</v>
-      </c>
-      <c r="O14" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" t="s">
-        <v>529</v>
-      </c>
-      <c r="C15" t="s">
-        <v>529</v>
-      </c>
-      <c r="D15" t="s">
-        <v>556</v>
-      </c>
-      <c r="F15" t="s">
-        <v>532</v>
-      </c>
-      <c r="G15" t="s">
-        <v>529</v>
-      </c>
-      <c r="L15" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" t="s">
-        <v>530</v>
-      </c>
-      <c r="C16" t="s">
-        <v>530</v>
-      </c>
-      <c r="D16" t="s">
-        <v>560</v>
-      </c>
-      <c r="F16" t="s">
-        <v>533</v>
-      </c>
-      <c r="G16" t="s">
-        <v>530</v>
-      </c>
-      <c r="L16" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" t="s">
-        <v>531</v>
-      </c>
-      <c r="C17" t="s">
-        <v>531</v>
-      </c>
-      <c r="D17" t="s">
-        <v>561</v>
-      </c>
-      <c r="F17" t="s">
-        <v>534</v>
-      </c>
-      <c r="G17" t="s">
-        <v>531</v>
-      </c>
-      <c r="L17" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" t="s">
-        <v>532</v>
-      </c>
-      <c r="C18" t="s">
-        <v>532</v>
-      </c>
-      <c r="D18" t="s">
-        <v>563</v>
-      </c>
-      <c r="F18" t="s">
-        <v>535</v>
-      </c>
-      <c r="G18" t="s">
-        <v>532</v>
-      </c>
-      <c r="L18" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" t="s">
-        <v>533</v>
-      </c>
-      <c r="C19" t="s">
-        <v>533</v>
-      </c>
-      <c r="D19" t="s">
-        <v>567</v>
-      </c>
-      <c r="F19" t="s">
-        <v>536</v>
-      </c>
-      <c r="G19" t="s">
-        <v>533</v>
-      </c>
-      <c r="L19" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" t="s">
-        <v>534</v>
-      </c>
-      <c r="C20" t="s">
-        <v>534</v>
-      </c>
-      <c r="D20" t="s">
-        <v>568</v>
-      </c>
-      <c r="F20" t="s">
-        <v>538</v>
-      </c>
-      <c r="G20" t="s">
-        <v>534</v>
-      </c>
-      <c r="L20" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" t="s">
-        <v>535</v>
-      </c>
-      <c r="C21" t="s">
-        <v>535</v>
-      </c>
-      <c r="D21" t="s">
-        <v>569</v>
-      </c>
-      <c r="F21" t="s">
-        <v>539</v>
-      </c>
-      <c r="G21" t="s">
-        <v>535</v>
-      </c>
-      <c r="L21" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" t="s">
-        <v>536</v>
-      </c>
-      <c r="C22" t="s">
-        <v>536</v>
-      </c>
-      <c r="D22" t="s">
-        <v>570</v>
-      </c>
-      <c r="F22" t="s">
-        <v>540</v>
-      </c>
-      <c r="G22" t="s">
-        <v>536</v>
-      </c>
-      <c r="L22" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" t="s">
-        <v>537</v>
-      </c>
-      <c r="C23" t="s">
-        <v>537</v>
-      </c>
-      <c r="D23" t="s">
-        <v>571</v>
-      </c>
-      <c r="F23" t="s">
-        <v>541</v>
-      </c>
-      <c r="G23" t="s">
-        <v>537</v>
-      </c>
-      <c r="L23" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" t="s">
-        <v>538</v>
-      </c>
-      <c r="C24" t="s">
-        <v>538</v>
-      </c>
-      <c r="F24" t="s">
-        <v>543</v>
-      </c>
-      <c r="G24" t="s">
-        <v>538</v>
-      </c>
-      <c r="L24" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" t="s">
-        <v>539</v>
-      </c>
-      <c r="C25" t="s">
-        <v>539</v>
-      </c>
-      <c r="F25" t="s">
-        <v>544</v>
-      </c>
-      <c r="G25" t="s">
-        <v>539</v>
-      </c>
-      <c r="L25" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" t="s">
-        <v>540</v>
-      </c>
-      <c r="C26" t="s">
-        <v>540</v>
-      </c>
-      <c r="F26" t="s">
-        <v>545</v>
-      </c>
-      <c r="G26" t="s">
-        <v>540</v>
-      </c>
-      <c r="L26" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" t="s">
-        <v>541</v>
-      </c>
-      <c r="C27" t="s">
-        <v>541</v>
-      </c>
-      <c r="F27" t="s">
-        <v>549</v>
-      </c>
-      <c r="G27" t="s">
-        <v>541</v>
-      </c>
-      <c r="L27" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" t="s">
-        <v>542</v>
-      </c>
-      <c r="C28" t="s">
-        <v>542</v>
-      </c>
-      <c r="F28" t="s">
-        <v>550</v>
-      </c>
-      <c r="G28" t="s">
-        <v>542</v>
-      </c>
-      <c r="L28" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" t="s">
-        <v>543</v>
-      </c>
-      <c r="C29" t="s">
-        <v>543</v>
-      </c>
-      <c r="F29" t="s">
-        <v>552</v>
-      </c>
-      <c r="G29" t="s">
-        <v>543</v>
-      </c>
-      <c r="L29" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" t="s">
-        <v>544</v>
-      </c>
-      <c r="C30" t="s">
-        <v>544</v>
-      </c>
-      <c r="F30" t="s">
-        <v>554</v>
-      </c>
-      <c r="G30" t="s">
-        <v>544</v>
-      </c>
-      <c r="L30" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" t="s">
-        <v>545</v>
-      </c>
-      <c r="C31" t="s">
-        <v>545</v>
-      </c>
-      <c r="F31" t="s">
-        <v>555</v>
-      </c>
-      <c r="G31" t="s">
-        <v>545</v>
-      </c>
-      <c r="L31" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" t="s">
-        <v>546</v>
-      </c>
-      <c r="C32" t="s">
-        <v>546</v>
-      </c>
-      <c r="F32" t="s">
-        <v>556</v>
-      </c>
-      <c r="G32" t="s">
-        <v>546</v>
-      </c>
-      <c r="L32" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" t="s">
-        <v>547</v>
-      </c>
-      <c r="C33" t="s">
-        <v>547</v>
-      </c>
-      <c r="F33" t="s">
-        <v>557</v>
-      </c>
-      <c r="G33" t="s">
-        <v>547</v>
-      </c>
-      <c r="L33" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" t="s">
-        <v>548</v>
-      </c>
-      <c r="C34" t="s">
-        <v>548</v>
-      </c>
-      <c r="F34" t="s">
-        <v>560</v>
-      </c>
-      <c r="G34" t="s">
-        <v>548</v>
-      </c>
-      <c r="L34" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" t="s">
-        <v>549</v>
-      </c>
-      <c r="C35" t="s">
-        <v>549</v>
-      </c>
-      <c r="F35" t="s">
-        <v>561</v>
-      </c>
-      <c r="G35" t="s">
-        <v>549</v>
-      </c>
-      <c r="L35" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" t="s">
-        <v>550</v>
-      </c>
-      <c r="C36" t="s">
-        <v>550</v>
-      </c>
-      <c r="F36" t="s">
-        <v>563</v>
-      </c>
-      <c r="G36" t="s">
-        <v>550</v>
-      </c>
-      <c r="L36" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" t="s">
-        <v>551</v>
-      </c>
-      <c r="C37" t="s">
-        <v>551</v>
-      </c>
-      <c r="F37" t="s">
-        <v>566</v>
-      </c>
-      <c r="G37" t="s">
-        <v>551</v>
-      </c>
-      <c r="L37" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" t="s">
-        <v>552</v>
-      </c>
-      <c r="C38" t="s">
-        <v>552</v>
-      </c>
-      <c r="F38" t="s">
-        <v>567</v>
-      </c>
-      <c r="G38" t="s">
-        <v>552</v>
-      </c>
-      <c r="L38" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" t="s">
-        <v>553</v>
-      </c>
-      <c r="C39" t="s">
-        <v>553</v>
-      </c>
-      <c r="F39" t="s">
-        <v>568</v>
-      </c>
-      <c r="G39" t="s">
-        <v>553</v>
-      </c>
-      <c r="L39" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" t="s">
-        <v>554</v>
-      </c>
-      <c r="C40" t="s">
-        <v>554</v>
-      </c>
-      <c r="F40" t="s">
-        <v>569</v>
-      </c>
-      <c r="G40" t="s">
-        <v>554</v>
-      </c>
-      <c r="L40" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41" t="s">
-        <v>555</v>
-      </c>
-      <c r="C41" t="s">
-        <v>555</v>
-      </c>
-      <c r="F41" t="s">
-        <v>570</v>
-      </c>
-      <c r="G41" t="s">
-        <v>555</v>
-      </c>
-      <c r="L41" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" t="s">
-        <v>556</v>
-      </c>
-      <c r="C42" t="s">
-        <v>556</v>
-      </c>
-      <c r="F42" t="s">
-        <v>571</v>
-      </c>
-      <c r="G42" t="s">
-        <v>556</v>
-      </c>
-      <c r="L42" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" t="s">
-        <v>557</v>
-      </c>
-      <c r="C43" t="s">
-        <v>557</v>
-      </c>
-      <c r="G43" t="s">
-        <v>557</v>
-      </c>
-      <c r="L43" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="A44" t="s">
-        <v>558</v>
-      </c>
-      <c r="C44" t="s">
-        <v>558</v>
-      </c>
-      <c r="G44" t="s">
-        <v>558</v>
-      </c>
-      <c r="L44" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="A45" t="s">
-        <v>559</v>
-      </c>
-      <c r="C45" t="s">
-        <v>559</v>
-      </c>
-      <c r="G45" t="s">
-        <v>559</v>
-      </c>
-      <c r="L45" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="A46" t="s">
-        <v>560</v>
-      </c>
-      <c r="C46" t="s">
-        <v>560</v>
-      </c>
-      <c r="G46" t="s">
-        <v>560</v>
-      </c>
-      <c r="L46" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" t="s">
-        <v>561</v>
-      </c>
-      <c r="C47" t="s">
-        <v>561</v>
-      </c>
-      <c r="G47" t="s">
-        <v>561</v>
-      </c>
-      <c r="L47" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" t="s">
-        <v>562</v>
-      </c>
-      <c r="C48" t="s">
-        <v>562</v>
-      </c>
-      <c r="G48" t="s">
-        <v>562</v>
-      </c>
-      <c r="L48" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="A49" t="s">
-        <v>563</v>
-      </c>
-      <c r="C49" t="s">
-        <v>563</v>
-      </c>
-      <c r="G49" t="s">
-        <v>563</v>
-      </c>
-      <c r="L49" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="A50" t="s">
-        <v>564</v>
-      </c>
-      <c r="C50" t="s">
-        <v>564</v>
-      </c>
-      <c r="G50" t="s">
-        <v>564</v>
-      </c>
-      <c r="L50" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" t="s">
-        <v>565</v>
-      </c>
-      <c r="C51" t="s">
-        <v>565</v>
-      </c>
-      <c r="G51" t="s">
-        <v>565</v>
-      </c>
-      <c r="L51" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12">
-      <c r="A52" t="s">
-        <v>566</v>
-      </c>
-      <c r="C52" t="s">
-        <v>566</v>
-      </c>
-      <c r="G52" t="s">
-        <v>566</v>
-      </c>
-      <c r="L52" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53" t="s">
-        <v>567</v>
-      </c>
-      <c r="C53" t="s">
-        <v>567</v>
-      </c>
-      <c r="G53" t="s">
-        <v>567</v>
-      </c>
-      <c r="L53" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
-      <c r="A54" t="s">
-        <v>568</v>
-      </c>
-      <c r="C54" t="s">
-        <v>568</v>
-      </c>
-      <c r="G54" t="s">
-        <v>568</v>
-      </c>
-      <c r="L54" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="A55" t="s">
-        <v>569</v>
-      </c>
-      <c r="C55" t="s">
-        <v>569</v>
-      </c>
-      <c r="G55" t="s">
-        <v>569</v>
-      </c>
-      <c r="L55" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="A56" t="s">
-        <v>570</v>
-      </c>
-      <c r="C56" t="s">
-        <v>570</v>
-      </c>
-      <c r="G56" t="s">
-        <v>570</v>
-      </c>
-      <c r="L56" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="A57" t="s">
-        <v>571</v>
-      </c>
-      <c r="C57" t="s">
-        <v>571</v>
-      </c>
-      <c r="G57" t="s">
-        <v>571</v>
-      </c>
-      <c r="L57" t="s">
-        <v>571</v>
+    <row r="8" spans="1:14">
+      <c r="B8" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>